<commit_message>
Refactoring BoardIndex. Split from BoardIndex classes EffectivityIndex, Orders.
</commit_message>
<xml_diff>
--- a/UML/Книга1.xlsx
+++ b/UML/Книга1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_MyProg\Boards\UML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AFBC1A-EC1A-418F-BBE9-E5A05E290E1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CFEEDF-8F72-40B4-87BB-9953150C4A9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{0D71F9EF-39D5-4BF9-BDF9-4866CAA684C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{0D71F9EF-39D5-4BF9-BDF9-4866CAA684C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Компоненты" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Условия" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="141">
   <si>
     <t>Установка названия</t>
   </si>
@@ -122,9 +122,6 @@
     <t>- + связь с любым рабочим местом</t>
   </si>
   <si>
-    <t>++</t>
-  </si>
-  <si>
     <t>CanbanBoard</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>Кол. карточек</t>
   </si>
   <si>
-    <t>+ исскуственный</t>
-  </si>
-  <si>
     <t>+ искусственный</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>+искуственный</t>
   </si>
   <si>
-    <t>+ искуственный</t>
-  </si>
-  <si>
     <t>Двойное создание сначала конвеер затем листья</t>
   </si>
   <si>
@@ -362,9 +353,6 @@
     <t>KM 164Cb            </t>
   </si>
   <si>
-    <t>KM 217Cb            </t>
-  </si>
-  <si>
     <t>KM 012CpR           </t>
   </si>
   <si>
@@ -480,6 +468,36 @@
   </si>
   <si>
     <t>11. pid</t>
+  </si>
+  <si>
+    <t>+ симв.тип=title</t>
+  </si>
+  <si>
+    <t>MFC1847087***       </t>
+  </si>
+  <si>
+    <t>MFC1847034***       </t>
+  </si>
+  <si>
+    <t>MFC1802012***       </t>
+  </si>
+  <si>
+    <t>MFC1802317***       </t>
+  </si>
+  <si>
+    <t>MFC1847164***       </t>
+  </si>
+  <si>
+    <t>MFC1847217***       </t>
+  </si>
+  <si>
+    <t>MFC180317***        </t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>KM 217Cb</t>
   </si>
 </sst>
 </file>
@@ -927,11 +945,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB0A29E-00BE-43A5-8916-8072B1B9736A}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="F14:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,77 +968,77 @@
         <v>10</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" t="s">
-        <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="N2" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1028,14 +1046,14 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>6</v>
@@ -1073,13 +1091,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>6</v>
@@ -1088,22 +1106,22 @@
         <v>6</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="N5" s="11" t="s">
         <v>6</v>
@@ -1117,11 +1135,11 @@
         <v>0</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>6</v>
@@ -1153,11 +1171,11 @@
         <v>4</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>6</v>
@@ -1192,16 +1210,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>6</v>
@@ -1228,7 +1246,7 @@
         <v>6</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1236,14 +1254,14 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>6</v>
@@ -1260,7 +1278,7 @@
         <v>6</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1276,7 +1294,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -1306,14 +1324,14 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -1325,7 +1343,7 @@
         <v>6</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N12" s="8"/>
     </row>
@@ -1334,14 +1352,14 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -1363,26 +1381,26 @@
         <v>7</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -1396,23 +1414,23 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I15" s="11" t="s">
         <v>6</v>
@@ -1424,7 +1442,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="15"/>
       <c r="N15" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1432,14 +1450,14 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -1458,16 +1476,16 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -1486,20 +1504,20 @@
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -1507,10 +1525,10 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -1518,14 +1536,14 @@
         <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F19" s="16"/>
       <c r="G19" s="8"/>
@@ -1545,11 +1563,11 @@
         <v>2</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>6</v>
@@ -1575,11 +1593,11 @@
         <v>3</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>11</v>
@@ -1599,7 +1617,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1613,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26E99DB-3EEB-4E34-A82F-9F316DBF632D}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,52 +1645,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
         <v>107</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" t="s">
         <v>108</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N1" t="s">
-        <v>111</v>
-      </c>
-      <c r="O1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1680,10 +1698,10 @@
         <v>1001</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D2" s="7">
         <v>1</v>
@@ -1720,10 +1738,10 @@
         <v>1002</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
@@ -1760,10 +1778,10 @@
         <v>1003</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
@@ -1800,10 +1818,10 @@
         <v>1004</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
@@ -1840,10 +1858,10 @@
         <v>1005</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
@@ -1880,10 +1898,10 @@
         <v>1006</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D7" s="7">
         <v>1</v>
@@ -1920,10 +1938,10 @@
         <v>1007</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
@@ -1960,10 +1978,10 @@
         <v>1008</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
@@ -2000,10 +2018,10 @@
         <v>1009</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
@@ -2040,10 +2058,10 @@
         <v>1010</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D11" s="7">
         <v>1</v>
@@ -2080,10 +2098,10 @@
         <v>1011</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D12" s="7">
         <v>1</v>
@@ -2120,10 +2138,10 @@
         <v>1012</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D13" s="7">
         <v>1</v>
@@ -2160,10 +2178,10 @@
         <v>1013</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D14" s="7">
         <v>1</v>
@@ -2200,10 +2218,10 @@
         <v>1014</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D15" s="7">
         <v>1</v>
@@ -2240,10 +2258,10 @@
         <v>1015</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D16" s="7">
         <v>1</v>
@@ -2280,10 +2298,10 @@
         <v>1016</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D17" s="7">
         <v>1</v>
@@ -2320,10 +2338,10 @@
         <v>1017</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D18" s="7">
         <v>1</v>
@@ -2360,10 +2378,10 @@
         <v>1018</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D19" s="7">
         <v>1</v>
@@ -2400,10 +2418,10 @@
         <v>1100</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D20" s="7">
         <v>1</v>
@@ -2440,10 +2458,10 @@
         <v>1101</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D21" s="7">
         <v>1</v>
@@ -2480,10 +2498,10 @@
         <v>1525</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D22" s="7">
         <v>1</v>
@@ -2520,10 +2538,10 @@
         <v>1902</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D23" s="7">
         <v>1</v>
@@ -2560,10 +2578,10 @@
         <v>1903</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D24" s="7">
         <v>1</v>
@@ -2600,10 +2618,10 @@
         <v>1904</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D25" s="7">
         <v>1</v>
@@ -2640,10 +2658,10 @@
         <v>1905</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D26" s="7">
         <v>1</v>
@@ -2680,10 +2698,10 @@
         <v>1906</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
@@ -2720,10 +2738,10 @@
         <v>1907</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
@@ -2760,10 +2778,10 @@
         <v>1908</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D29" s="7">
         <v>1</v>
@@ -2800,10 +2818,10 @@
         <v>3001</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D30" s="7">
         <v>1</v>
@@ -2840,10 +2858,10 @@
         <v>3002</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D31" s="7">
         <v>1</v>
@@ -2880,10 +2898,10 @@
         <v>3003</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D32" s="7">
         <v>1</v>
@@ -2920,10 +2938,10 @@
         <v>3101</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D33" s="7">
         <v>1</v>
@@ -2949,7 +2967,7 @@
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
       <c r="M33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="N33" s="7">
         <v>0</v>
@@ -2963,10 +2981,10 @@
         <v>3102</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D34" s="7">
         <v>1</v>
@@ -2992,7 +3010,7 @@
       <c r="K34" s="7"/>
       <c r="L34" s="7"/>
       <c r="M34" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="N34" s="7">
         <v>0</v>
@@ -3006,10 +3024,10 @@
         <v>3103</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D35" s="7">
         <v>1</v>
@@ -3046,10 +3064,10 @@
         <v>3104</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D36" s="7">
         <v>1</v>
@@ -3087,7 +3105,7 @@
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D37" s="7">
         <v>1</v>
@@ -3125,7 +3143,7 @@
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D38" s="7">
         <v>1</v>
@@ -3163,7 +3181,7 @@
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D39" s="7">
         <v>1</v>
@@ -3201,7 +3219,7 @@
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D40" s="7">
         <v>1</v>
@@ -3238,10 +3256,10 @@
         <v>3301</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D41" s="7">
         <v>1</v>
@@ -3278,10 +3296,10 @@
         <v>3302</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D42" s="7">
         <v>1</v>
@@ -3318,10 +3336,10 @@
         <v>3303</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D43" s="7">
         <v>1</v>
@@ -3358,10 +3376,10 @@
         <v>4012</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D44" s="7">
         <v>1</v>
@@ -3398,10 +3416,10 @@
         <v>4023</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D45" s="7">
         <v>1</v>
@@ -3440,12 +3458,239 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF9E5ACF-4EA5-47AA-AE3C-DC64E837A0F9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>4023</v>
+      </c>
+      <c r="C1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>4023</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>4012</v>
+      </c>
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>4012</v>
+      </c>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4012</v>
+      </c>
+      <c r="C5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>1902</v>
+      </c>
+      <c r="C6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1903</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>1904</v>
+      </c>
+      <c r="C8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>1905</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1906</v>
+      </c>
+      <c r="C10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1907</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>1525</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>1910</v>
+      </c>
+      <c r="C13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1911</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>1912</v>
+      </c>
+      <c r="C15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>1913</v>
+      </c>
+      <c r="C16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>3024</v>
+      </c>
+      <c r="C17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>3024</v>
+      </c>
+      <c r="C18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>3024</v>
+      </c>
+      <c r="C19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>